<commit_message>
Excel reading bug not resolved.
</commit_message>
<xml_diff>
--- a/src/import-data/import-subjects.xlsx
+++ b/src/import-data/import-subjects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jankoj\Desktop\WMS.React\src\import-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E29F08-7F8A-414B-B47D-35254AB8F23F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836CFD48-275C-40FF-90A8-FAC1A9DC973B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22716" yWindow="1176" windowWidth="21600" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,8 +84,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,370 +370,372 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2">
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1">
         <v>4</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="1">
         <f t="shared" ref="A3:A20" si="0">A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3">
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1">
         <v>2</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4">
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
         <v>2</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5">
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
         <v>3</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6">
+      <c r="A6" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1">
         <v>1</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7">
+      <c r="A7" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
         <v>33</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8">
+      <c r="A8" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1">
         <v>33</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9">
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1">
         <v>4</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10">
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1">
         <v>4</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11">
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1">
         <v>4</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12">
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1">
         <v>4</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13">
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1">
         <v>78</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14">
-        <v>5</v>
-      </c>
-      <c r="E14">
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1">
+        <v>5</v>
+      </c>
+      <c r="E14" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15">
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1">
         <v>44</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16">
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="1">
         <v>3</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17">
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="1">
         <v>2</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18">
+      <c r="B18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="1">
         <v>9</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19">
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1">
         <v>9</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20">
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="1">
         <v>9</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="1">
         <v>5</v>
       </c>
     </row>

</xml_diff>